<commit_message>
ICA done, saved as .csv files
</commit_message>
<xml_diff>
--- a/reports/data.xlsx
+++ b/reports/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D173"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>length</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ic_removed</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -463,7 +468,12 @@
         <v>32</v>
       </c>
       <c r="D2" t="n">
-        <v>65500</v>
+        <v>64000</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>[0, 2, 30]</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -479,7 +489,12 @@
         <v>32</v>
       </c>
       <c r="D3" t="n">
-        <v>68000</v>
+        <v>66500</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 6, 10]</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -495,7 +510,12 @@
         <v>32</v>
       </c>
       <c r="D4" t="n">
-        <v>61500</v>
+        <v>60000</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>[1, 7, 21]</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -511,7 +531,12 @@
         <v>32</v>
       </c>
       <c r="D5" t="n">
-        <v>63500</v>
+        <v>62000</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>[0, 1, 27, 6]</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -527,7 +552,12 @@
         <v>32</v>
       </c>
       <c r="D6" t="n">
-        <v>66000</v>
+        <v>64500</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>[21, 25]</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -543,7 +573,12 @@
         <v>32</v>
       </c>
       <c r="D7" t="n">
-        <v>66000</v>
+        <v>64500</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>[0, 23, 24, 17]</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -559,7 +594,12 @@
         <v>32</v>
       </c>
       <c r="D8" t="n">
-        <v>71500</v>
+        <v>70000</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>[12, 7, 2, 27]</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -575,7 +615,12 @@
         <v>32</v>
       </c>
       <c r="D9" t="n">
-        <v>66500</v>
+        <v>65000</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 9]</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -591,7 +636,12 @@
         <v>32</v>
       </c>
       <c r="D10" t="n">
-        <v>66500</v>
+        <v>65000</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>[25, 23, 1, 14]</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -607,7 +657,12 @@
         <v>32</v>
       </c>
       <c r="D11" t="n">
-        <v>66000</v>
+        <v>64500</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>[0, 4, 16, 25, 30]</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -623,7 +678,12 @@
         <v>32</v>
       </c>
       <c r="D12" t="n">
-        <v>66000</v>
+        <v>64500</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>[2, 11]</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -639,7 +699,12 @@
         <v>32</v>
       </c>
       <c r="D13" t="n">
-        <v>66000</v>
+        <v>64500</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>[0, 1, 8, 14, 25]</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -655,7 +720,12 @@
         <v>32</v>
       </c>
       <c r="D14" t="n">
-        <v>65500</v>
+        <v>64000</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>[5, 16, 27]</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -671,7 +741,12 @@
         <v>32</v>
       </c>
       <c r="D15" t="n">
-        <v>66000</v>
+        <v>64500</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>[12, 4, 6]</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -687,7 +762,12 @@
         <v>32</v>
       </c>
       <c r="D16" t="n">
-        <v>67000</v>
+        <v>65500</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>[1, 28, 29, 30]</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -703,7 +783,12 @@
         <v>32</v>
       </c>
       <c r="D17" t="n">
-        <v>67500</v>
+        <v>66000</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>[0, 2, 11, 13, 26]</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -719,7 +804,12 @@
         <v>32</v>
       </c>
       <c r="D18" t="n">
-        <v>62000</v>
+        <v>60500</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>[0, 10, 15, 16, 25]</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -735,7 +825,12 @@
         <v>32</v>
       </c>
       <c r="D19" t="n">
-        <v>66000</v>
+        <v>64500</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>[1, 2, 5, 6, 7, 27]</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -751,7 +846,12 @@
         <v>32</v>
       </c>
       <c r="D20" t="n">
-        <v>66500</v>
+        <v>65000</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>[6, 29]</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -767,7 +867,12 @@
         <v>32</v>
       </c>
       <c r="D21" t="n">
-        <v>65000</v>
+        <v>63500</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>[0, 2, 17]</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -783,7 +888,12 @@
         <v>32</v>
       </c>
       <c r="D22" t="n">
-        <v>66000</v>
+        <v>64500</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>[0, 1, 3, 5, 14, 11, 12]</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -799,7 +909,12 @@
         <v>32</v>
       </c>
       <c r="D23" t="n">
-        <v>66500</v>
+        <v>65000</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>[0, 1, 30, 20, 28]</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -808,14 +923,19 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>S15_Pre_EC1_EEG</t>
+          <t>S16_post_EC1</t>
         </is>
       </c>
       <c r="C24" t="n">
         <v>32</v>
       </c>
       <c r="D24" t="n">
-        <v>66000</v>
+        <v>65000</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>[10, 24]</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -824,14 +944,19 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>S15_Pre_EO1_EEG</t>
+          <t>S16_post_EO1</t>
         </is>
       </c>
       <c r="C25" t="n">
         <v>32</v>
       </c>
       <c r="D25" t="n">
-        <v>66500</v>
+        <v>65000</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>[0, 1, 3, 12]</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -840,14 +965,19 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>S16_post_EC1</t>
+          <t>S16-Pre-EC1_EEG</t>
         </is>
       </c>
       <c r="C26" t="n">
         <v>32</v>
       </c>
       <c r="D26" t="n">
-        <v>66500</v>
+        <v>65500</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>[0, 7, 9]</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -856,14 +986,19 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>S16_post_EO1</t>
+          <t>S16-Pre-EO1_EEG</t>
         </is>
       </c>
       <c r="C27" t="n">
         <v>32</v>
       </c>
       <c r="D27" t="n">
-        <v>66500</v>
+        <v>65000</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 4]</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -872,14 +1007,19 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>S16-Pre-EC1_EEG</t>
+          <t>S17-Post-EO1</t>
         </is>
       </c>
       <c r="C28" t="n">
         <v>32</v>
       </c>
       <c r="D28" t="n">
-        <v>67000</v>
+        <v>64500</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>[0, 1, 12, 26]</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -888,14 +1028,19 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>S16-Pre-EO1_EEG</t>
+          <t>S17-Post_EC1</t>
         </is>
       </c>
       <c r="C29" t="n">
         <v>32</v>
       </c>
       <c r="D29" t="n">
-        <v>66500</v>
+        <v>64500</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>[0, 11]</t>
+        </is>
       </c>
     </row>
     <row r="30">
@@ -904,14 +1049,19 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>S17-Post-EO1</t>
+          <t>S17-Pre_EC1_EEG</t>
         </is>
       </c>
       <c r="C30" t="n">
         <v>32</v>
       </c>
       <c r="D30" t="n">
-        <v>66000</v>
+        <v>64500</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>[0, 7, 6]</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -920,14 +1070,19 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>S17-Post_EC1</t>
+          <t>S17-Pre_EO1_EEG</t>
         </is>
       </c>
       <c r="C31" t="n">
         <v>32</v>
       </c>
       <c r="D31" t="n">
-        <v>66000</v>
+        <v>64500</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>[0, 4, 30]</t>
+        </is>
       </c>
     </row>
     <row r="32">
@@ -936,14 +1091,19 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>S17-Pre_EC1_EEG</t>
+          <t>S18_post_EC1</t>
         </is>
       </c>
       <c r="C32" t="n">
         <v>32</v>
       </c>
       <c r="D32" t="n">
-        <v>66000</v>
+        <v>64500</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>[1, 26, 28]</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -952,14 +1112,19 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>S17-Pre_EO1_EEG</t>
+          <t>S18_Post_EO1_EEG</t>
         </is>
       </c>
       <c r="C33" t="n">
         <v>32</v>
       </c>
       <c r="D33" t="n">
-        <v>66000</v>
+        <v>64500</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>[0, 3, 22, 24]</t>
+        </is>
       </c>
     </row>
     <row r="34">
@@ -968,14 +1133,19 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>S18_post_EC1</t>
+          <t>S19_post_EC1</t>
         </is>
       </c>
       <c r="C34" t="n">
         <v>32</v>
       </c>
       <c r="D34" t="n">
-        <v>66000</v>
+        <v>64500</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>[0, 19, 10, 16, 17, 21, 30, 27]</t>
+        </is>
       </c>
     </row>
     <row r="35">
@@ -984,14 +1154,19 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>S18_Post_EO1_EEG</t>
+          <t>S19_Post_EO1</t>
         </is>
       </c>
       <c r="C35" t="n">
         <v>32</v>
       </c>
       <c r="D35" t="n">
-        <v>66000</v>
+        <v>65500</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>[0, 1, 7, 29]</t>
+        </is>
       </c>
     </row>
     <row r="36">
@@ -1000,14 +1175,19 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>S18-pre_EC1_EEG</t>
+          <t>S19_EC1_EEG</t>
         </is>
       </c>
       <c r="C36" t="n">
         <v>32</v>
       </c>
       <c r="D36" t="n">
-        <v>67000</v>
+        <v>64500</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>[0, 1, 14, 18, 23]</t>
+        </is>
       </c>
     </row>
     <row r="37">
@@ -1016,14 +1196,19 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>S18-pre_EO1_EEG</t>
+          <t>S19_EO1_EEG</t>
         </is>
       </c>
       <c r="C37" t="n">
         <v>32</v>
       </c>
       <c r="D37" t="n">
-        <v>66000</v>
+        <v>65000</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>[0, 1, 12, 14, 19, 25, 28]</t>
+        </is>
       </c>
     </row>
     <row r="38">
@@ -1032,14 +1217,19 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>S19_post_EC1</t>
+          <t>S1 post_EC1_EEG</t>
         </is>
       </c>
       <c r="C38" t="n">
         <v>32</v>
       </c>
       <c r="D38" t="n">
-        <v>66000</v>
+        <v>61500</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 4]</t>
+        </is>
       </c>
     </row>
     <row r="39">
@@ -1048,14 +1238,19 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>S19_Post_EO1</t>
+          <t>S1 post_EO1_EEG</t>
         </is>
       </c>
       <c r="C39" t="n">
         <v>32</v>
       </c>
       <c r="D39" t="n">
-        <v>67000</v>
+        <v>62000</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 4, 14, 30, 22]</t>
+        </is>
       </c>
     </row>
     <row r="40">
@@ -1064,14 +1259,19 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>S19_EC1_EEG</t>
+          <t>S1_Pre-EO1_EEG</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D40" t="n">
-        <v>66000</v>
+        <v>60000</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>[0, 23, 24, 25, 28]</t>
+        </is>
       </c>
     </row>
     <row r="41">
@@ -1080,14 +1280,19 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>S19_EO1_EEG</t>
+          <t>S20_Post_EC1</t>
         </is>
       </c>
       <c r="C41" t="n">
         <v>32</v>
       </c>
       <c r="D41" t="n">
-        <v>66500</v>
+        <v>64000</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>[0, 10]</t>
+        </is>
       </c>
     </row>
     <row r="42">
@@ -1096,14 +1301,19 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>S1 post_EC1_EEG</t>
+          <t>S20_post_EO1</t>
         </is>
       </c>
       <c r="C42" t="n">
         <v>32</v>
       </c>
       <c r="D42" t="n">
-        <v>63000</v>
+        <v>64500</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>[0, 1, 2]</t>
+        </is>
       </c>
     </row>
     <row r="43">
@@ -1112,14 +1322,19 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>S1 post_EO1_EEG</t>
+          <t>S20_pre_EC1_EEG</t>
         </is>
       </c>
       <c r="C43" t="n">
         <v>32</v>
       </c>
       <c r="D43" t="n">
-        <v>63500</v>
+        <v>65500</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>[0, 4, 20, 23]</t>
+        </is>
       </c>
     </row>
     <row r="44">
@@ -1128,14 +1343,19 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>S1_Pre-EC1_EEG</t>
+          <t>S20_pre_EO1_EEG</t>
         </is>
       </c>
       <c r="C44" t="n">
         <v>32</v>
       </c>
       <c r="D44" t="n">
-        <v>64000</v>
+        <v>64500</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>[0, 2, 3, 12, 15, 21]</t>
+        </is>
       </c>
     </row>
     <row r="45">
@@ -1144,14 +1364,19 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>S1_Pre-EO1_EEG</t>
+          <t>S21_post_EC1_EEG</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D45" t="n">
-        <v>61500</v>
+        <v>64000</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>[0, 10, 3, 27]</t>
+        </is>
       </c>
     </row>
     <row r="46">
@@ -1160,14 +1385,19 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>S20_Post_EC1</t>
+          <t>S21_post_EO1_EEG</t>
         </is>
       </c>
       <c r="C46" t="n">
         <v>32</v>
       </c>
       <c r="D46" t="n">
-        <v>65500</v>
+        <v>65000</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 14]</t>
+        </is>
       </c>
     </row>
     <row r="47">
@@ -1176,14 +1406,19 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>S20_post_EO1</t>
+          <t>S22_Post_EC1_EEG</t>
         </is>
       </c>
       <c r="C47" t="n">
         <v>32</v>
       </c>
       <c r="D47" t="n">
-        <v>66000</v>
+        <v>64500</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>[0, 2, 7, 25, 29]</t>
+        </is>
       </c>
     </row>
     <row r="48">
@@ -1192,14 +1427,19 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>S20_pre_EC1_EEG</t>
+          <t>S22_Post_EO1_EEG</t>
         </is>
       </c>
       <c r="C48" t="n">
         <v>32</v>
       </c>
       <c r="D48" t="n">
-        <v>67000</v>
+        <v>65500</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>[0, 1, 3, 26]</t>
+        </is>
       </c>
     </row>
     <row r="49">
@@ -1208,14 +1448,19 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>S20_pre_EO1_EEG</t>
+          <t>S22_Pre_EC1_EEG</t>
         </is>
       </c>
       <c r="C49" t="n">
         <v>32</v>
       </c>
       <c r="D49" t="n">
-        <v>66000</v>
+        <v>64500</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>[0, 3, 8, 11, 28]</t>
+        </is>
       </c>
     </row>
     <row r="50">
@@ -1224,14 +1469,19 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>S21_post_EC1_EEG</t>
+          <t>S22_Pre_EO1_EEG</t>
         </is>
       </c>
       <c r="C50" t="n">
         <v>32</v>
       </c>
       <c r="D50" t="n">
-        <v>65500</v>
+        <v>64500</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>[0, 5, 2, 7, 23, 26]</t>
+        </is>
       </c>
     </row>
     <row r="51">
@@ -1240,14 +1490,19 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>S21_post_EO1_EEG</t>
+          <t>S23_PreEC1_EEG</t>
         </is>
       </c>
       <c r="C51" t="n">
         <v>32</v>
       </c>
       <c r="D51" t="n">
-        <v>66500</v>
+        <v>64000</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>[0, 1, 12, 28, 29]</t>
+        </is>
       </c>
     </row>
     <row r="52">
@@ -1256,14 +1511,19 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>S22_Post_EC1_EEG</t>
+          <t>S23_PreEO1_EEG</t>
         </is>
       </c>
       <c r="C52" t="n">
         <v>32</v>
       </c>
       <c r="D52" t="n">
-        <v>66000</v>
+        <v>64000</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>[1, 11, 3, 7, 20, 30]</t>
+        </is>
       </c>
     </row>
     <row r="53">
@@ -1272,14 +1532,19 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>S22_Post_EO1_EEG</t>
+          <t>S24_Post_EC1</t>
         </is>
       </c>
       <c r="C53" t="n">
         <v>32</v>
       </c>
       <c r="D53" t="n">
-        <v>67000</v>
+        <v>64000</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>[0, 11, 21, 24]</t>
+        </is>
       </c>
     </row>
     <row r="54">
@@ -1288,14 +1553,19 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>S22_Pre_EC1_EEG</t>
+          <t>S24_post_EO1</t>
         </is>
       </c>
       <c r="C54" t="n">
         <v>32</v>
       </c>
       <c r="D54" t="n">
-        <v>66000</v>
+        <v>65500</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>[0, 2, 8, 24]</t>
+        </is>
       </c>
     </row>
     <row r="55">
@@ -1304,14 +1574,19 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>S22_Pre_EO1_EEG</t>
+          <t>S24_pre_EC1</t>
         </is>
       </c>
       <c r="C55" t="n">
         <v>32</v>
       </c>
       <c r="D55" t="n">
-        <v>66000</v>
+        <v>64000</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>[0, 1, 15, 24]</t>
+        </is>
       </c>
     </row>
     <row r="56">
@@ -1320,14 +1595,19 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>S23_PreEC1_EEG</t>
+          <t>S25_Pre_EC1_EEG</t>
         </is>
       </c>
       <c r="C56" t="n">
         <v>32</v>
       </c>
       <c r="D56" t="n">
-        <v>65500</v>
+        <v>64500</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>[0, 1, 3]</t>
+        </is>
       </c>
     </row>
     <row r="57">
@@ -1336,14 +1616,19 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>S23_PreEO1_EEG</t>
+          <t>S25_Pre_EO1_EEG</t>
         </is>
       </c>
       <c r="C57" t="n">
         <v>32</v>
       </c>
       <c r="D57" t="n">
-        <v>65500</v>
+        <v>64500</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 4]</t>
+        </is>
       </c>
     </row>
     <row r="58">
@@ -1352,14 +1637,19 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>S24_Post_EC1</t>
+          <t>S27_post_EC1</t>
         </is>
       </c>
       <c r="C58" t="n">
         <v>32</v>
       </c>
       <c r="D58" t="n">
-        <v>65500</v>
+        <v>65000</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>[2, 12, 20]</t>
+        </is>
       </c>
     </row>
     <row r="59">
@@ -1368,14 +1658,19 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>S24_post_EO1</t>
+          <t>S27_post_EO1</t>
         </is>
       </c>
       <c r="C59" t="n">
         <v>32</v>
       </c>
       <c r="D59" t="n">
-        <v>67000</v>
+        <v>64500</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>[0, 5, 13]</t>
+        </is>
       </c>
     </row>
     <row r="60">
@@ -1384,14 +1679,19 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>S24_pre_EC1</t>
+          <t>S27_pre_EC1_EEG</t>
         </is>
       </c>
       <c r="C60" t="n">
         <v>32</v>
       </c>
       <c r="D60" t="n">
-        <v>65500</v>
+        <v>64000</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>[1, 14, 22, 6]</t>
+        </is>
       </c>
     </row>
     <row r="61">
@@ -1400,14 +1700,19 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>S24_pre_EO1</t>
+          <t>S27_pre_EO1_EEG</t>
         </is>
       </c>
       <c r="C61" t="n">
         <v>32</v>
       </c>
       <c r="D61" t="n">
-        <v>66000</v>
+        <v>64000</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>[0, 23, 25]</t>
+        </is>
       </c>
     </row>
     <row r="62">
@@ -1416,14 +1721,19 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>S25_Post_EC1_EEG</t>
+          <t>S29_Pre_EC1_EEG</t>
         </is>
       </c>
       <c r="C62" t="n">
         <v>32</v>
       </c>
       <c r="D62" t="n">
-        <v>66500</v>
+        <v>64500</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>[0, 2, 7]</t>
+        </is>
       </c>
     </row>
     <row r="63">
@@ -1432,14 +1742,19 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>S25_Post_EO1_EEG</t>
+          <t>S29_Pre_EO1_EEG</t>
         </is>
       </c>
       <c r="C63" t="n">
         <v>32</v>
       </c>
       <c r="D63" t="n">
-        <v>66000</v>
+        <v>64000</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>[3, 9, 30]</t>
+        </is>
       </c>
     </row>
     <row r="64">
@@ -1448,14 +1763,19 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>S25_Pre_EC1_EEG</t>
+          <t>S2-Post-_EC1_EEG</t>
         </is>
       </c>
       <c r="C64" t="n">
         <v>32</v>
       </c>
       <c r="D64" t="n">
-        <v>66000</v>
+        <v>64500</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>[2, 29, 30]</t>
+        </is>
       </c>
     </row>
     <row r="65">
@@ -1464,14 +1784,19 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>S25_Pre_EO1_EEG</t>
+          <t>S2-Post_EO1_EEG</t>
         </is>
       </c>
       <c r="C65" t="n">
         <v>32</v>
       </c>
       <c r="D65" t="n">
-        <v>66000</v>
+        <v>64500</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 5]</t>
+        </is>
       </c>
     </row>
     <row r="66">
@@ -1480,14 +1805,19 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>S26_pre_EC1_EEG</t>
+          <t>S2-Pre-_EC1_EEG</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="D66" t="n">
-        <v>65500</v>
+        <v>59500</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>[0, 1, 8, 30]</t>
+        </is>
       </c>
     </row>
     <row r="67">
@@ -1496,14 +1826,19 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>S26_pre_EO1_EEG</t>
+          <t>S2-Pre_EO_EEG</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="D67" t="n">
-        <v>66000</v>
+        <v>60000</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 23]</t>
+        </is>
       </c>
     </row>
     <row r="68">
@@ -1512,14 +1847,19 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>S27_post_EC1</t>
+          <t>S30_EC1_post_EEG</t>
         </is>
       </c>
       <c r="C68" t="n">
         <v>32</v>
       </c>
       <c r="D68" t="n">
-        <v>66500</v>
+        <v>64500</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 5, 9, 20]</t>
+        </is>
       </c>
     </row>
     <row r="69">
@@ -1528,14 +1868,19 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>S27_post_EO1</t>
+          <t>S30_EO1_post_EEG</t>
         </is>
       </c>
       <c r="C69" t="n">
         <v>32</v>
       </c>
       <c r="D69" t="n">
-        <v>66000</v>
+        <v>64000</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 7]</t>
+        </is>
       </c>
     </row>
     <row r="70">
@@ -1544,14 +1889,19 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>S27_pre_EC1_EEG</t>
+          <t>S30_Pre_EC1</t>
         </is>
       </c>
       <c r="C70" t="n">
         <v>32</v>
       </c>
       <c r="D70" t="n">
-        <v>65500</v>
+        <v>64500</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 5, 8, 9]</t>
+        </is>
       </c>
     </row>
     <row r="71">
@@ -1560,14 +1910,19 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>S27_pre_EO1_EEG</t>
+          <t>S30_Pre_EO1</t>
         </is>
       </c>
       <c r="C71" t="n">
         <v>32</v>
       </c>
       <c r="D71" t="n">
-        <v>65500</v>
+        <v>64000</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 7]</t>
+        </is>
       </c>
     </row>
     <row r="72">
@@ -1576,14 +1931,19 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>S29_EC1_Post_EEG</t>
+          <t>S31_EC1_post_EEG</t>
         </is>
       </c>
       <c r="C72" t="n">
         <v>32</v>
       </c>
       <c r="D72" t="n">
-        <v>66000</v>
+        <v>63000</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>[0, 1, 11, 26]</t>
+        </is>
       </c>
     </row>
     <row r="73">
@@ -1592,14 +1952,19 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>S29_EO1Post_EEG</t>
+          <t>S31_EO1_post_EEG</t>
         </is>
       </c>
       <c r="C73" t="n">
         <v>32</v>
       </c>
       <c r="D73" t="n">
-        <v>65500</v>
+        <v>63000</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 6, 12, 28]</t>
+        </is>
       </c>
     </row>
     <row r="74">
@@ -1608,14 +1973,19 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>S29_Pre_EC1_EEG</t>
+          <t>S31_pre_EC1_EEG</t>
         </is>
       </c>
       <c r="C74" t="n">
         <v>32</v>
       </c>
       <c r="D74" t="n">
-        <v>66000</v>
+        <v>64000</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>[0, 1, 5, 20, 30]</t>
+        </is>
       </c>
     </row>
     <row r="75">
@@ -1624,14 +1994,19 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>S29_Pre_EO1_EEG</t>
+          <t>S31_pre_EO1_EEG</t>
         </is>
       </c>
       <c r="C75" t="n">
         <v>32</v>
       </c>
       <c r="D75" t="n">
-        <v>65500</v>
+        <v>64000</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>[0, 1, 18]</t>
+        </is>
       </c>
     </row>
     <row r="76">
@@ -1640,14 +2015,19 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>S2-Post-_EC1_EEG</t>
+          <t>S32_EC1_pre_EEG</t>
         </is>
       </c>
       <c r="C76" t="n">
         <v>32</v>
       </c>
       <c r="D76" t="n">
-        <v>66000</v>
+        <v>64000</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>[0, 18, 20, 26, 28]</t>
+        </is>
       </c>
     </row>
     <row r="77">
@@ -1656,14 +2036,19 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>S2-Post_EO1_EEG</t>
+          <t>S32_EO1_pre_EEG</t>
         </is>
       </c>
       <c r="C77" t="n">
         <v>32</v>
       </c>
       <c r="D77" t="n">
-        <v>66000</v>
+        <v>64000</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>[0, 18, 24]</t>
+        </is>
       </c>
     </row>
     <row r="78">
@@ -1672,14 +2057,19 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>S2-Pre-_EC1_EEG</t>
+          <t>S32_EC1_post_EEG</t>
         </is>
       </c>
       <c r="C78" t="n">
         <v>32</v>
       </c>
       <c r="D78" t="n">
-        <v>61000</v>
+        <v>64000</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>[0, 4, 21, 24, 30]</t>
+        </is>
       </c>
     </row>
     <row r="79">
@@ -1688,14 +2078,19 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>S2-Pre_EO_EEG</t>
+          <t>S32_EO1_post_EEG</t>
         </is>
       </c>
       <c r="C79" t="n">
         <v>32</v>
       </c>
       <c r="D79" t="n">
-        <v>61500</v>
+        <v>64000</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>[0, 2, 18, 27]</t>
+        </is>
       </c>
     </row>
     <row r="80">
@@ -1704,14 +2099,19 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>S30_EC1_post_EEG</t>
+          <t>S33_Pre_EC1_EEG</t>
         </is>
       </c>
       <c r="C80" t="n">
         <v>32</v>
       </c>
       <c r="D80" t="n">
-        <v>66000</v>
+        <v>64500</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>[0, 5, 10, 23]</t>
+        </is>
       </c>
     </row>
     <row r="81">
@@ -1720,14 +2120,19 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>S30_EO1_post_EEG</t>
+          <t>S33_Pre_EO1_EEG</t>
         </is>
       </c>
       <c r="C81" t="n">
         <v>32</v>
       </c>
       <c r="D81" t="n">
-        <v>65500</v>
+        <v>64500</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>[0, 13, 15]</t>
+        </is>
       </c>
     </row>
     <row r="82">
@@ -1736,14 +2141,19 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>S30_Pre_EC1</t>
+          <t>S36_Post_EC1_EEG</t>
         </is>
       </c>
       <c r="C82" t="n">
         <v>32</v>
       </c>
       <c r="D82" t="n">
-        <v>66000</v>
+        <v>64500</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>[0, 1, 18, 19, 20, 25, 17]</t>
+        </is>
       </c>
     </row>
     <row r="83">
@@ -1752,14 +2162,19 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>S30_Pre_EO1</t>
+          <t>S36_Post_EO1_EEG</t>
         </is>
       </c>
       <c r="C83" t="n">
         <v>32</v>
       </c>
       <c r="D83" t="n">
-        <v>65500</v>
+        <v>64500</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>[0, 1, 10, 13, 15, 24, 25]</t>
+        </is>
       </c>
     </row>
     <row r="84">
@@ -1768,7 +2183,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>S31_EC1_post_EEG</t>
+          <t>S36_pre_Ec1_EEG</t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -1776,6 +2191,11 @@
       </c>
       <c r="D84" t="n">
         <v>64500</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 6, 8, 16, 22]</t>
+        </is>
       </c>
     </row>
     <row r="85">
@@ -1784,14 +2204,19 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>S31_EO1_post_EEG</t>
+          <t>S36_pre_Eo1_EEG</t>
         </is>
       </c>
       <c r="C85" t="n">
         <v>32</v>
       </c>
       <c r="D85" t="n">
-        <v>64500</v>
+        <v>60000</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 9, 27, 29]</t>
+        </is>
       </c>
     </row>
     <row r="86">
@@ -1800,14 +2225,19 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>S31_pre_EC1_EEG</t>
+          <t>S37_EC1_post_EEG</t>
         </is>
       </c>
       <c r="C86" t="n">
         <v>32</v>
       </c>
       <c r="D86" t="n">
-        <v>65500</v>
+        <v>64000</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>[0, 6, 19, 26]</t>
+        </is>
       </c>
     </row>
     <row r="87">
@@ -1816,14 +2246,19 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>S31_pre_EO1_EEG</t>
+          <t>S37_EO1_post_EEG</t>
         </is>
       </c>
       <c r="C87" t="n">
         <v>32</v>
       </c>
       <c r="D87" t="n">
-        <v>65500</v>
+        <v>64500</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>[0, 3, 22, 23]</t>
+        </is>
       </c>
     </row>
     <row r="88">
@@ -1832,14 +2267,19 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>S32_EC1_pre_EEG</t>
+          <t>S38_EC1_post_EEG</t>
         </is>
       </c>
       <c r="C88" t="n">
         <v>32</v>
       </c>
       <c r="D88" t="n">
-        <v>65500</v>
+        <v>64500</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>[0, 1, 10, 29]</t>
+        </is>
       </c>
     </row>
     <row r="89">
@@ -1848,14 +2288,19 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>S32_EO1_pre_EEG</t>
+          <t>S38_EO1_post_EEG</t>
         </is>
       </c>
       <c r="C89" t="n">
         <v>32</v>
       </c>
       <c r="D89" t="n">
-        <v>65500</v>
+        <v>64500</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 4, 18]</t>
+        </is>
       </c>
     </row>
     <row r="90">
@@ -1864,14 +2309,19 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>S32_EC1_post_EEG</t>
+          <t>S38_Pre_EC1__EEG</t>
         </is>
       </c>
       <c r="C90" t="n">
         <v>32</v>
       </c>
       <c r="D90" t="n">
-        <v>65500</v>
+        <v>64500</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>[0, 12, 25, 30, 29]</t>
+        </is>
       </c>
     </row>
     <row r="91">
@@ -1880,14 +2330,19 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>S32_EO1_post_EEG</t>
+          <t>S38_Pre_EO1_EEG</t>
         </is>
       </c>
       <c r="C91" t="n">
         <v>32</v>
       </c>
       <c r="D91" t="n">
-        <v>65500</v>
+        <v>64000</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>[0, 1, 4, 19, 25]</t>
+        </is>
       </c>
     </row>
     <row r="92">
@@ -1896,14 +2351,19 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>S33_Post_EC1_EEG</t>
+          <t>S39_Pre_EO1_EEG</t>
         </is>
       </c>
       <c r="C92" t="n">
         <v>32</v>
       </c>
       <c r="D92" t="n">
-        <v>65500</v>
+        <v>64500</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>[0]</t>
+        </is>
       </c>
     </row>
     <row r="93">
@@ -1912,14 +2372,19 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>S33_Post_EO1_EEG</t>
+          <t>S3-post_EC1_EEG</t>
         </is>
       </c>
       <c r="C93" t="n">
         <v>32</v>
       </c>
       <c r="D93" t="n">
-        <v>65500</v>
+        <v>60000</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>[3, 13, 21, 28]</t>
+        </is>
       </c>
     </row>
     <row r="94">
@@ -1928,14 +2393,19 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>S33_Pre_EC1_EEG</t>
+          <t>S3-Post_EO1_EEG</t>
         </is>
       </c>
       <c r="C94" t="n">
         <v>32</v>
       </c>
       <c r="D94" t="n">
-        <v>66000</v>
+        <v>62000</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 5, 19]</t>
+        </is>
       </c>
     </row>
     <row r="95">
@@ -1944,14 +2414,19 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>S33_Pre_EO1_EEG</t>
+          <t>S3-pre_EC1</t>
         </is>
       </c>
       <c r="C95" t="n">
         <v>32</v>
       </c>
       <c r="D95" t="n">
-        <v>66000</v>
+        <v>62000</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>[0, 5, 28]</t>
+        </is>
       </c>
     </row>
     <row r="96">
@@ -1960,7 +2435,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>S35-PostEC1_EEG</t>
+          <t>S3-pre_EC2_EEG</t>
         </is>
       </c>
       <c r="C96" t="n">
@@ -1968,6 +2443,11 @@
       </c>
       <c r="D96" t="n">
         <v>65500</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>[0, 1, 18, 23, 25]</t>
+        </is>
       </c>
     </row>
     <row r="97">
@@ -1976,14 +2456,19 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>S35-PostEO1_EEG</t>
+          <t>S3-pre_EO1_EEG</t>
         </is>
       </c>
       <c r="C97" t="n">
         <v>32</v>
       </c>
       <c r="D97" t="n">
-        <v>66000</v>
+        <v>65000</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 11, 28, 19]</t>
+        </is>
       </c>
     </row>
     <row r="98">
@@ -1992,14 +2477,19 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>S35_pre_Ec1_EEG</t>
+          <t>S3-pre_EO2_EEG</t>
         </is>
       </c>
       <c r="C98" t="n">
         <v>32</v>
       </c>
       <c r="D98" t="n">
-        <v>66000</v>
+        <v>65500</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 9, 16, 27]</t>
+        </is>
       </c>
     </row>
     <row r="99">
@@ -2008,14 +2498,19 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>S35_pre_Eo1_EEG</t>
+          <t>S41__EO1_pre_EEG</t>
         </is>
       </c>
       <c r="C99" t="n">
         <v>32</v>
       </c>
       <c r="D99" t="n">
-        <v>65500</v>
+        <v>65000</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 9, 22, 29]</t>
+        </is>
       </c>
     </row>
     <row r="100">
@@ -2024,14 +2519,19 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>S36_Post_EC1_EEG</t>
+          <t>S43_EO1Post_EEG</t>
         </is>
       </c>
       <c r="C100" t="n">
         <v>32</v>
       </c>
       <c r="D100" t="n">
-        <v>66000</v>
+        <v>64500</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>[0, 3, 25, 26]</t>
+        </is>
       </c>
     </row>
     <row r="101">
@@ -2040,14 +2540,19 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>S36_Post_EO1_EEG</t>
+          <t>S43_PostEC1</t>
         </is>
       </c>
       <c r="C101" t="n">
         <v>32</v>
       </c>
       <c r="D101" t="n">
-        <v>66000</v>
+        <v>64500</v>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>[20, 25, 29]</t>
+        </is>
       </c>
     </row>
     <row r="102">
@@ -2056,14 +2561,19 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>S36_pre_Ec1_EEG</t>
+          <t>S43_PreEC1_EEG</t>
         </is>
       </c>
       <c r="C102" t="n">
         <v>32</v>
       </c>
       <c r="D102" t="n">
-        <v>66000</v>
+        <v>65000</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>[2, 15, 26, 27, 23]</t>
+        </is>
       </c>
     </row>
     <row r="103">
@@ -2072,14 +2582,19 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>S36_pre_Eo1_EEG</t>
+          <t>S43_PreEO1_EEG</t>
         </is>
       </c>
       <c r="C103" t="n">
         <v>32</v>
       </c>
       <c r="D103" t="n">
-        <v>61500</v>
+        <v>64500</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>[0, 1, 3, 18, 16, 19, 21]</t>
+        </is>
       </c>
     </row>
     <row r="104">
@@ -2088,14 +2603,19 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>S37_EC1_post_EEG</t>
+          <t>S46_EC1_post_EEG</t>
         </is>
       </c>
       <c r="C104" t="n">
         <v>32</v>
       </c>
       <c r="D104" t="n">
-        <v>65500</v>
+        <v>78000</v>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>[0]</t>
+        </is>
       </c>
     </row>
     <row r="105">
@@ -2104,14 +2624,19 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>S37_EO1_post_EEG</t>
+          <t>S49_pre_EC1_EEG</t>
         </is>
       </c>
       <c r="C105" t="n">
         <v>32</v>
       </c>
       <c r="D105" t="n">
-        <v>66000</v>
+        <v>65000</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 4, 11, 24, 6, 28]</t>
+        </is>
       </c>
     </row>
     <row r="106">
@@ -2120,14 +2645,19 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>S37_EC1_Pre_EEG</t>
+          <t>S49_pre_EO1_EEG</t>
         </is>
       </c>
       <c r="C106" t="n">
         <v>32</v>
       </c>
       <c r="D106" t="n">
-        <v>66000</v>
+        <v>64500</v>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>[3, 6, 13, 16, 28, 7]</t>
+        </is>
       </c>
     </row>
     <row r="107">
@@ -2136,14 +2666,19 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>S37_EO1_Pre_EEG</t>
+          <t>S4-post_EC1_EEG</t>
         </is>
       </c>
       <c r="C107" t="n">
         <v>32</v>
       </c>
       <c r="D107" t="n">
-        <v>66500</v>
+        <v>61000</v>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>[0, 1, 22, 30]</t>
+        </is>
       </c>
     </row>
     <row r="108">
@@ -2152,14 +2687,19 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>S38_EC1_post_EEG</t>
+          <t>S4-post_EO1_EEG</t>
         </is>
       </c>
       <c r="C108" t="n">
         <v>32</v>
       </c>
       <c r="D108" t="n">
-        <v>66000</v>
+        <v>62000</v>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>[0, 1, 13, 30]</t>
+        </is>
       </c>
     </row>
     <row r="109">
@@ -2168,14 +2708,19 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>S38_EO1_post_EEG</t>
+          <t>S4-pre_EC1_EEG</t>
         </is>
       </c>
       <c r="C109" t="n">
         <v>32</v>
       </c>
       <c r="D109" t="n">
-        <v>66000</v>
+        <v>61500</v>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>[0, 1, 3, 30]</t>
+        </is>
       </c>
     </row>
     <row r="110">
@@ -2184,14 +2729,19 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>S38_Pre_EC1__EEG</t>
+          <t>S4-pre_EO1_EEG</t>
         </is>
       </c>
       <c r="C110" t="n">
         <v>32</v>
       </c>
       <c r="D110" t="n">
-        <v>66000</v>
+        <v>61500</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 5]</t>
+        </is>
       </c>
     </row>
     <row r="111">
@@ -2200,7 +2750,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>S38_Pre_EO1_EEG</t>
+          <t>S5-post EC1_EEG</t>
         </is>
       </c>
       <c r="C111" t="n">
@@ -2208,6 +2758,11 @@
       </c>
       <c r="D111" t="n">
         <v>65500</v>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>[7, 5, 29]</t>
+        </is>
       </c>
     </row>
     <row r="112">
@@ -2216,7 +2771,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>S39-Post_EC1_EEG</t>
+          <t>S5-post EO1_EEG</t>
         </is>
       </c>
       <c r="C112" t="n">
@@ -2224,6 +2779,11 @@
       </c>
       <c r="D112" t="n">
         <v>66000</v>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>[0, 3, 10]</t>
+        </is>
       </c>
     </row>
     <row r="113">
@@ -2232,14 +2792,19 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>S39-Post_EO1_EEG</t>
+          <t>S5_EC1_EEG</t>
         </is>
       </c>
       <c r="C113" t="n">
         <v>32</v>
       </c>
       <c r="D113" t="n">
-        <v>66000</v>
+        <v>65000</v>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>[0, 1, 11, 27, 24, 4]</t>
+        </is>
       </c>
     </row>
     <row r="114">
@@ -2248,14 +2813,19 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>S39_Pre_EC1_EEG</t>
+          <t>S5_EO1_EEG</t>
         </is>
       </c>
       <c r="C114" t="n">
         <v>32</v>
       </c>
       <c r="D114" t="n">
-        <v>65500</v>
+        <v>65000</v>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>[0, 2, 8, 26]</t>
+        </is>
       </c>
     </row>
     <row r="115">
@@ -2264,14 +2834,19 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>S39_Pre_EO1_EEG</t>
+          <t>S6-pre_EC1_EEG</t>
         </is>
       </c>
       <c r="C115" t="n">
         <v>32</v>
       </c>
       <c r="D115" t="n">
-        <v>66000</v>
+        <v>64500</v>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>[0, 10, 20]</t>
+        </is>
       </c>
     </row>
     <row r="116">
@@ -2280,14 +2855,19 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>S3-post_EC1_EEG</t>
+          <t>S6-pre_EO1_EEG</t>
         </is>
       </c>
       <c r="C116" t="n">
         <v>32</v>
       </c>
       <c r="D116" t="n">
-        <v>61500</v>
+        <v>64500</v>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>[0, 1, 17]</t>
+        </is>
       </c>
     </row>
     <row r="117">
@@ -2296,14 +2876,19 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>S3-Post_EO1_EEG</t>
+          <t>S7-post-EC1_EEG</t>
         </is>
       </c>
       <c r="C117" t="n">
         <v>32</v>
       </c>
       <c r="D117" t="n">
-        <v>63500</v>
+        <v>64000</v>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>[3, 12, 18, 22, 29]</t>
+        </is>
       </c>
     </row>
     <row r="118">
@@ -2312,14 +2897,19 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>S3-pre_EC1</t>
+          <t>S7-post-EO1_EEG</t>
         </is>
       </c>
       <c r="C118" t="n">
         <v>32</v>
       </c>
       <c r="D118" t="n">
-        <v>63500</v>
+        <v>64500</v>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>[0, 1, 11, 30]</t>
+        </is>
       </c>
     </row>
     <row r="119">
@@ -2328,14 +2918,19 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>S3-pre_EC2_EEG</t>
+          <t>S8_Post_EO1_EEG</t>
         </is>
       </c>
       <c r="C119" t="n">
         <v>32</v>
       </c>
       <c r="D119" t="n">
-        <v>67000</v>
+        <v>64500</v>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 4, 5]</t>
+        </is>
       </c>
     </row>
     <row r="120">
@@ -2344,14 +2939,19 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>S3-pre_EO1_EEG</t>
+          <t>S8-EC1pre_EEG</t>
         </is>
       </c>
       <c r="C120" t="n">
         <v>32</v>
       </c>
       <c r="D120" t="n">
-        <v>66500</v>
+        <v>62000</v>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 15, 16, 18, 5, 8]</t>
+        </is>
       </c>
     </row>
     <row r="121">
@@ -2360,846 +2960,19 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>S3-pre_EO2_EEG</t>
+          <t>S9-post-EO1_EEG</t>
         </is>
       </c>
       <c r="C121" t="n">
         <v>32</v>
       </c>
       <c r="D121" t="n">
-        <v>67000</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" s="1" t="n">
-        <v>120</v>
-      </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>S40_EC_Post_EEG</t>
-        </is>
-      </c>
-      <c r="C122" t="n">
-        <v>32</v>
-      </c>
-      <c r="D122" t="n">
-        <v>66000</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" s="1" t="n">
-        <v>121</v>
-      </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>S40_EO1_post_EEG</t>
-        </is>
-      </c>
-      <c r="C123" t="n">
-        <v>32</v>
-      </c>
-      <c r="D123" t="n">
-        <v>65500</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" s="1" t="n">
-        <v>122</v>
-      </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>S40_EC_Pre_EEG</t>
-        </is>
-      </c>
-      <c r="C124" t="n">
-        <v>32</v>
-      </c>
-      <c r="D124" t="n">
-        <v>65500</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" s="1" t="n">
-        <v>123</v>
-      </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>S40_EO_pre_EEG</t>
-        </is>
-      </c>
-      <c r="C125" t="n">
-        <v>32</v>
-      </c>
-      <c r="D125" t="n">
-        <v>66000</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" s="1" t="n">
-        <v>124</v>
-      </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>S41_EC1_post_EEG</t>
-        </is>
-      </c>
-      <c r="C126" t="n">
-        <v>32</v>
-      </c>
-      <c r="D126" t="n">
-        <v>65500</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" s="1" t="n">
-        <v>125</v>
-      </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>S41_EO1_post_EEG</t>
-        </is>
-      </c>
-      <c r="C127" t="n">
-        <v>32</v>
-      </c>
-      <c r="D127" t="n">
-        <v>65500</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" s="1" t="n">
-        <v>126</v>
-      </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>S41_EC1_pre_EEG</t>
-        </is>
-      </c>
-      <c r="C128" t="n">
-        <v>32</v>
-      </c>
-      <c r="D128" t="n">
-        <v>65000</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" s="1" t="n">
-        <v>127</v>
-      </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>S41__EO1_pre_EEG</t>
-        </is>
-      </c>
-      <c r="C129" t="n">
-        <v>32</v>
-      </c>
-      <c r="D129" t="n">
-        <v>66500</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" s="1" t="n">
-        <v>128</v>
-      </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>S42_EC1PostBilal_EEG</t>
-        </is>
-      </c>
-      <c r="C130" t="n">
-        <v>32</v>
-      </c>
-      <c r="D130" t="n">
-        <v>67000</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" s="1" t="n">
-        <v>129</v>
-      </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>S42_EO1PostBilal</t>
-        </is>
-      </c>
-      <c r="C131" t="n">
-        <v>32</v>
-      </c>
-      <c r="D131" t="n">
-        <v>72000</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" s="1" t="n">
-        <v>130</v>
-      </c>
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>S42_pre_EO1</t>
-        </is>
-      </c>
-      <c r="C132" t="n">
-        <v>32</v>
-      </c>
-      <c r="D132" t="n">
-        <v>66500</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" s="1" t="n">
-        <v>131</v>
-      </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>S42_Prre_EC1</t>
-        </is>
-      </c>
-      <c r="C133" t="n">
-        <v>32</v>
-      </c>
-      <c r="D133" t="n">
-        <v>62000</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" s="1" t="n">
-        <v>132</v>
-      </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>S43_EO1Post_EEG</t>
-        </is>
-      </c>
-      <c r="C134" t="n">
-        <v>32</v>
-      </c>
-      <c r="D134" t="n">
-        <v>66000</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" s="1" t="n">
-        <v>133</v>
-      </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>S43_PostEC1</t>
-        </is>
-      </c>
-      <c r="C135" t="n">
-        <v>32</v>
-      </c>
-      <c r="D135" t="n">
-        <v>66000</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" s="1" t="n">
-        <v>134</v>
-      </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>S43_PreEC1_EEG</t>
-        </is>
-      </c>
-      <c r="C136" t="n">
-        <v>32</v>
-      </c>
-      <c r="D136" t="n">
-        <v>66500</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" s="1" t="n">
-        <v>135</v>
-      </c>
-      <c r="B137" t="inlineStr">
-        <is>
-          <t>S43_PreEO1_EEG</t>
-        </is>
-      </c>
-      <c r="C137" t="n">
-        <v>32</v>
-      </c>
-      <c r="D137" t="n">
-        <v>66000</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" s="1" t="n">
-        <v>136</v>
-      </c>
-      <c r="B138" t="inlineStr">
-        <is>
-          <t>S44_EC1_post_EEG</t>
-        </is>
-      </c>
-      <c r="C138" t="n">
-        <v>32</v>
-      </c>
-      <c r="D138" t="n">
-        <v>65500</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" s="1" t="n">
-        <v>137</v>
-      </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>S44_EO1_post_EEG</t>
-        </is>
-      </c>
-      <c r="C139" t="n">
-        <v>32</v>
-      </c>
-      <c r="D139" t="n">
-        <v>66500</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" s="1" t="n">
-        <v>138</v>
-      </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>S44_EC1_pre_EEG</t>
-        </is>
-      </c>
-      <c r="C140" t="n">
-        <v>32</v>
-      </c>
-      <c r="D140" t="n">
-        <v>64500</v>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" s="1" t="n">
-        <v>139</v>
-      </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>S44_EO1_pre_EEG</t>
-        </is>
-      </c>
-      <c r="C141" t="n">
-        <v>32</v>
-      </c>
-      <c r="D141" t="n">
         <v>64000</v>
       </c>
-    </row>
-    <row r="142">
-      <c r="A142" s="1" t="n">
-        <v>140</v>
-      </c>
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>S45_Post_EC1_EEG</t>
-        </is>
-      </c>
-      <c r="C142" t="n">
-        <v>32</v>
-      </c>
-      <c r="D142" t="n">
-        <v>66000</v>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" s="1" t="n">
-        <v>141</v>
-      </c>
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>S45_Post_EO1_EEG</t>
-        </is>
-      </c>
-      <c r="C143" t="n">
-        <v>32</v>
-      </c>
-      <c r="D143" t="n">
-        <v>65500</v>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" s="1" t="n">
-        <v>142</v>
-      </c>
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>S45_EC1_Pre_EEG</t>
-        </is>
-      </c>
-      <c r="C144" t="n">
-        <v>32</v>
-      </c>
-      <c r="D144" t="n">
-        <v>66500</v>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" s="1" t="n">
-        <v>143</v>
-      </c>
-      <c r="B145" t="inlineStr">
-        <is>
-          <t>S45_EO1_pre_EEG</t>
-        </is>
-      </c>
-      <c r="C145" t="n">
-        <v>32</v>
-      </c>
-      <c r="D145" t="n">
-        <v>66000</v>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" s="1" t="n">
-        <v>144</v>
-      </c>
-      <c r="B146" t="inlineStr">
-        <is>
-          <t>S46_EC1_post_EEG</t>
-        </is>
-      </c>
-      <c r="C146" t="n">
-        <v>32</v>
-      </c>
-      <c r="D146" t="n">
-        <v>79500</v>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" s="1" t="n">
-        <v>145</v>
-      </c>
-      <c r="B147" t="inlineStr">
-        <is>
-          <t>S46_EO1_post_EEG</t>
-        </is>
-      </c>
-      <c r="C147" t="n">
-        <v>32</v>
-      </c>
-      <c r="D147" t="n">
-        <v>66000</v>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" s="1" t="n">
-        <v>146</v>
-      </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>S46_Pre_EC1</t>
-        </is>
-      </c>
-      <c r="C148" t="n">
-        <v>32</v>
-      </c>
-      <c r="D148" t="n">
-        <v>66000</v>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" s="1" t="n">
-        <v>147</v>
-      </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>S46_Pre_EO1</t>
-        </is>
-      </c>
-      <c r="C149" t="n">
-        <v>32</v>
-      </c>
-      <c r="D149" t="n">
-        <v>66000</v>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" s="1" t="n">
-        <v>148</v>
-      </c>
-      <c r="B150" t="inlineStr">
-        <is>
-          <t>S47_pre_EC1_EEG</t>
-        </is>
-      </c>
-      <c r="C150" t="n">
-        <v>32</v>
-      </c>
-      <c r="D150" t="n">
-        <v>67500</v>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" s="1" t="n">
-        <v>149</v>
-      </c>
-      <c r="B151" t="inlineStr">
-        <is>
-          <t>S47_pre_EO1_EEG</t>
-        </is>
-      </c>
-      <c r="C151" t="n">
-        <v>32</v>
-      </c>
-      <c r="D151" t="n">
-        <v>66500</v>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" s="1" t="n">
-        <v>150</v>
-      </c>
-      <c r="B152" t="inlineStr">
-        <is>
-          <t>S49_pre_EC1_EEG</t>
-        </is>
-      </c>
-      <c r="C152" t="n">
-        <v>32</v>
-      </c>
-      <c r="D152" t="n">
-        <v>66500</v>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" s="1" t="n">
-        <v>151</v>
-      </c>
-      <c r="B153" t="inlineStr">
-        <is>
-          <t>S49_pre_EO1_EEG</t>
-        </is>
-      </c>
-      <c r="C153" t="n">
-        <v>32</v>
-      </c>
-      <c r="D153" t="n">
-        <v>66000</v>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" s="1" t="n">
-        <v>152</v>
-      </c>
-      <c r="B154" t="inlineStr">
-        <is>
-          <t>S4-post_EC1_EEG</t>
-        </is>
-      </c>
-      <c r="C154" t="n">
-        <v>32</v>
-      </c>
-      <c r="D154" t="n">
-        <v>62500</v>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" s="1" t="n">
-        <v>153</v>
-      </c>
-      <c r="B155" t="inlineStr">
-        <is>
-          <t>S4-post_EO1_EEG</t>
-        </is>
-      </c>
-      <c r="C155" t="n">
-        <v>32</v>
-      </c>
-      <c r="D155" t="n">
-        <v>63500</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" s="1" t="n">
-        <v>154</v>
-      </c>
-      <c r="B156" t="inlineStr">
-        <is>
-          <t>S4-pre_EC1_EEG</t>
-        </is>
-      </c>
-      <c r="C156" t="n">
-        <v>32</v>
-      </c>
-      <c r="D156" t="n">
-        <v>63000</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" s="1" t="n">
-        <v>155</v>
-      </c>
-      <c r="B157" t="inlineStr">
-        <is>
-          <t>S4-pre_EO1_EEG</t>
-        </is>
-      </c>
-      <c r="C157" t="n">
-        <v>32</v>
-      </c>
-      <c r="D157" t="n">
-        <v>63000</v>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" s="1" t="n">
-        <v>156</v>
-      </c>
-      <c r="B158" t="inlineStr">
-        <is>
-          <t>S5-post EC1_EEG</t>
-        </is>
-      </c>
-      <c r="C158" t="n">
-        <v>32</v>
-      </c>
-      <c r="D158" t="n">
-        <v>67000</v>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" s="1" t="n">
-        <v>157</v>
-      </c>
-      <c r="B159" t="inlineStr">
-        <is>
-          <t>S5-post EO1_EEG</t>
-        </is>
-      </c>
-      <c r="C159" t="n">
-        <v>32</v>
-      </c>
-      <c r="D159" t="n">
-        <v>67500</v>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" s="1" t="n">
-        <v>158</v>
-      </c>
-      <c r="B160" t="inlineStr">
-        <is>
-          <t>S5_EC1_EEG</t>
-        </is>
-      </c>
-      <c r="C160" t="n">
-        <v>32</v>
-      </c>
-      <c r="D160" t="n">
-        <v>66500</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" s="1" t="n">
-        <v>159</v>
-      </c>
-      <c r="B161" t="inlineStr">
-        <is>
-          <t>S5_EO1_EEG</t>
-        </is>
-      </c>
-      <c r="C161" t="n">
-        <v>32</v>
-      </c>
-      <c r="D161" t="n">
-        <v>66500</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" s="1" t="n">
-        <v>160</v>
-      </c>
-      <c r="B162" t="inlineStr">
-        <is>
-          <t>S6-pre_EC1_EEG</t>
-        </is>
-      </c>
-      <c r="C162" t="n">
-        <v>32</v>
-      </c>
-      <c r="D162" t="n">
-        <v>66000</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" s="1" t="n">
-        <v>161</v>
-      </c>
-      <c r="B163" t="inlineStr">
-        <is>
-          <t>S6-pre_EO1_EEG</t>
-        </is>
-      </c>
-      <c r="C163" t="n">
-        <v>32</v>
-      </c>
-      <c r="D163" t="n">
-        <v>66000</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" s="1" t="n">
-        <v>162</v>
-      </c>
-      <c r="B164" t="inlineStr">
-        <is>
-          <t>S7-post-EC1_EEG</t>
-        </is>
-      </c>
-      <c r="C164" t="n">
-        <v>32</v>
-      </c>
-      <c r="D164" t="n">
-        <v>65500</v>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" s="1" t="n">
-        <v>163</v>
-      </c>
-      <c r="B165" t="inlineStr">
-        <is>
-          <t>S7-post-EO1_EEG</t>
-        </is>
-      </c>
-      <c r="C165" t="n">
-        <v>32</v>
-      </c>
-      <c r="D165" t="n">
-        <v>66000</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" s="1" t="n">
-        <v>164</v>
-      </c>
-      <c r="B166" t="inlineStr">
-        <is>
-          <t>S8_Post_EC1_EEG</t>
-        </is>
-      </c>
-      <c r="C166" t="n">
-        <v>32</v>
-      </c>
-      <c r="D166" t="n">
-        <v>66000</v>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" s="1" t="n">
-        <v>165</v>
-      </c>
-      <c r="B167" t="inlineStr">
-        <is>
-          <t>S8_Post_EO1_EEG</t>
-        </is>
-      </c>
-      <c r="C167" t="n">
-        <v>32</v>
-      </c>
-      <c r="D167" t="n">
-        <v>66000</v>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" s="1" t="n">
-        <v>166</v>
-      </c>
-      <c r="B168" t="inlineStr">
-        <is>
-          <t>S8-EC1pre_EEG</t>
-        </is>
-      </c>
-      <c r="C168" t="n">
-        <v>32</v>
-      </c>
-      <c r="D168" t="n">
-        <v>63500</v>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" s="1" t="n">
-        <v>167</v>
-      </c>
-      <c r="B169" t="inlineStr">
-        <is>
-          <t>S8-EO1pre_EEG</t>
-        </is>
-      </c>
-      <c r="C169" t="n">
-        <v>32</v>
-      </c>
-      <c r="D169" t="n">
-        <v>63000</v>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" s="1" t="n">
-        <v>168</v>
-      </c>
-      <c r="B170" t="inlineStr">
-        <is>
-          <t>S9-post-EC1_EEG</t>
-        </is>
-      </c>
-      <c r="C170" t="n">
-        <v>32</v>
-      </c>
-      <c r="D170" t="n">
-        <v>65500</v>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" s="1" t="n">
-        <v>169</v>
-      </c>
-      <c r="B171" t="inlineStr">
-        <is>
-          <t>S9-post-EO1_EEG</t>
-        </is>
-      </c>
-      <c r="C171" t="n">
-        <v>32</v>
-      </c>
-      <c r="D171" t="n">
-        <v>65500</v>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" s="1" t="n">
-        <v>170</v>
-      </c>
-      <c r="B172" t="inlineStr">
-        <is>
-          <t>S9-Pre_EC1</t>
-        </is>
-      </c>
-      <c r="C172" t="n">
-        <v>32</v>
-      </c>
-      <c r="D172" t="n">
-        <v>64000</v>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" s="1" t="n">
-        <v>171</v>
-      </c>
-      <c r="B173" t="inlineStr">
-        <is>
-          <t>S9-Pre_EO1</t>
-        </is>
-      </c>
-      <c r="C173" t="n">
-        <v>32</v>
-      </c>
-      <c r="D173" t="n">
-        <v>64000</v>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 7, 14, 18]</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>